<commit_message>
Resolve import issues for N1 workflow
</commit_message>
<xml_diff>
--- a/Demo/msms_out_malG9120min_fluxconf.xlsx
+++ b/Demo/msms_out_malG9120min_fluxconf.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raaisa/Dropbox/Elucidata/corna_manuscript/Ipython_notebooks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raaisa/Documents/NA_Correction/Demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{9261E43D-C611-244B-8FB7-5632BA48DE75}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CB91DF-A28E-5441-A8AF-ED9A6B2EC04D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="msms_out_malG9120min_fluxconf" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId3"/>
+    <pivotCache cacheId="26" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="66">
   <si>
     <t>Component Name</t>
   </si>
@@ -220,11 +220,14 @@
   <si>
     <t>StdDev of Fractional enrichment</t>
   </si>
+  <si>
+    <t>Correct Fractional enrichment</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2042,7 +2045,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="43647.619338657409" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="61">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="43647.619338657409" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="61" xr:uid="{00000000-000A-0000-FFFF-FFFF05000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:E1048576" sheet="Sheet1"/>
   </cacheSource>
@@ -2563,7 +2566,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable1" cacheId="26" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="I8:W14" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField showAll="0"/>
@@ -3316,14 +3319,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U61"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:S1048576"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1:U1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="20.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
@@ -7293,15 +7299,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="29.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="28.33203125" bestFit="1" customWidth="1"/>
@@ -7341,6 +7349,9 @@
         <v>10</v>
       </c>
       <c r="E1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -7360,6 +7371,13 @@
       <c r="E2">
         <v>0.99987559329964903</v>
       </c>
+      <c r="F2">
+        <v>0.99987559329964903</v>
+      </c>
+      <c r="G2">
+        <f>IF(F2=E2,1,0)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -7377,6 +7395,13 @@
       <c r="E3">
         <v>0</v>
       </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G61" si="0">IF(F3=E3,1,0)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -7394,6 +7419,13 @@
       <c r="E4">
         <v>0</v>
       </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -7411,6 +7443,13 @@
       <c r="E5">
         <v>1.2440670035033499E-4</v>
       </c>
+      <c r="F5">
+        <v>1.2440670035033499E-4</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -7428,6 +7467,13 @@
       <c r="E6">
         <v>0</v>
       </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -7445,6 +7491,13 @@
       <c r="E7">
         <v>0.38659293648259502</v>
       </c>
+      <c r="F7">
+        <v>0.38659293648259502</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -7462,6 +7515,13 @@
       <c r="E8">
         <v>4.8347880633958999E-2</v>
       </c>
+      <c r="F8">
+        <v>4.8347880633958999E-2</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="J8" s="2" t="s">
         <v>60</v>
       </c>
@@ -7482,6 +7542,13 @@
       <c r="E9">
         <v>0.22661565457201499</v>
       </c>
+      <c r="F9">
+        <v>0.22661565457201499</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="J9" t="s">
         <v>25</v>
       </c>
@@ -7523,6 +7590,13 @@
       <c r="E10">
         <v>0.25930531812389201</v>
       </c>
+      <c r="F10">
+        <v>0.25930531812389201</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="I10" s="2" t="s">
         <v>57</v>
       </c>
@@ -7578,6 +7652,13 @@
       </c>
       <c r="E11">
         <v>7.9138210187537195E-2</v>
+      </c>
+      <c r="F11">
+        <v>7.9138210187537195E-2</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>22</v>
@@ -7637,6 +7718,13 @@
       <c r="E12">
         <v>0.99858492370061502</v>
       </c>
+      <c r="F12">
+        <v>0.99858492370061502</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="I12" s="3" t="s">
         <v>46</v>
       </c>
@@ -7694,6 +7782,13 @@
       </c>
       <c r="E13">
         <v>1.41507629938425E-3</v>
+      </c>
+      <c r="F13">
+        <v>1.41507629938425E-3</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>58</v>
@@ -7729,6 +7824,13 @@
       <c r="E14">
         <v>0</v>
       </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="I14" s="3" t="s">
         <v>59</v>
       </c>
@@ -7787,6 +7889,13 @@
       <c r="E15">
         <v>0</v>
       </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -7804,6 +7913,13 @@
       <c r="E16">
         <v>0</v>
       </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -7821,6 +7937,13 @@
       <c r="E17">
         <v>0.41725678831329399</v>
       </c>
+      <c r="F17">
+        <v>0.41725678831329399</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -7838,6 +7961,13 @@
       <c r="E18">
         <v>4.3953532040359303E-2</v>
       </c>
+      <c r="F18">
+        <v>4.3953532040359303E-2</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -7855,6 +7985,13 @@
       <c r="E19">
         <v>0.22769102462430299</v>
       </c>
+      <c r="F19">
+        <v>0.22769102462430299</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
@@ -7872,6 +8009,13 @@
       <c r="E20">
         <v>0.23415193276908</v>
       </c>
+      <c r="F20">
+        <v>0.23415193276908</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="I20" s="4"/>
       <c r="J20" s="4" t="s">
         <v>25</v>
@@ -7910,6 +8054,13 @@
       <c r="E21">
         <v>7.6946722252962896E-2</v>
       </c>
+      <c r="F21">
+        <v>7.6946722252962896E-2</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="I21" s="5" t="s">
         <v>57</v>
       </c>
@@ -7960,6 +8111,13 @@
       <c r="E22">
         <v>1</v>
       </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="I22" s="3" t="s">
         <v>46</v>
       </c>
@@ -8010,6 +8168,13 @@
       <c r="E23">
         <v>0</v>
       </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
@@ -8027,6 +8192,13 @@
       <c r="E24">
         <v>0</v>
       </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
@@ -8044,6 +8216,13 @@
       <c r="E25">
         <v>0</v>
       </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
@@ -8061,6 +8240,13 @@
       <c r="E26">
         <v>0</v>
       </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
@@ -8078,6 +8264,13 @@
       <c r="E27">
         <v>0.44211096678059902</v>
       </c>
+      <c r="F27">
+        <v>0.44211096678059902</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
@@ -8095,6 +8288,13 @@
       <c r="E28">
         <v>3.8663241437531901E-2</v>
       </c>
+      <c r="F28">
+        <v>3.8663241437531901E-2</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
@@ -8112,6 +8312,13 @@
       <c r="E29">
         <v>0.215199792938125</v>
       </c>
+      <c r="F29">
+        <v>0.215199792938125</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
@@ -8129,6 +8336,13 @@
       <c r="E30">
         <v>0.226903118748533</v>
       </c>
+      <c r="F30">
+        <v>0.226903118748533</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
@@ -8146,6 +8360,13 @@
       <c r="E31">
         <v>7.7122880095209706E-2</v>
       </c>
+      <c r="F31">
+        <v>7.7122880095209706E-2</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
@@ -8163,8 +8384,15 @@
       <c r="E32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -8180,8 +8408,15 @@
       <c r="E33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -8197,8 +8432,15 @@
       <c r="E34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -8214,8 +8456,15 @@
       <c r="E35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -8231,8 +8480,15 @@
       <c r="E36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>20</v>
       </c>
@@ -8248,8 +8504,15 @@
       <c r="E37">
         <v>0.51811252605674896</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37">
+        <v>0.51811252605674896</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>29</v>
       </c>
@@ -8265,8 +8528,15 @@
       <c r="E38">
         <v>3.8799642231361897E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38">
+        <v>3.8799642231361897E-2</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>33</v>
       </c>
@@ -8282,8 +8552,15 @@
       <c r="E39">
         <v>0.19583602759510499</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39">
+        <v>0.19583602759510499</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -8299,8 +8576,15 @@
       <c r="E40">
         <v>0.185222371292488</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40">
+        <v>0.185222371292488</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -8316,8 +8600,15 @@
       <c r="E41">
         <v>6.2029432824295003E-2</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41">
+        <v>6.2029432824295003E-2</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>20</v>
       </c>
@@ -8333,8 +8624,15 @@
       <c r="E42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>29</v>
       </c>
@@ -8350,8 +8648,15 @@
       <c r="E43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>33</v>
       </c>
@@ -8367,8 +8672,15 @@
       <c r="E44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>37</v>
       </c>
@@ -8384,8 +8696,15 @@
       <c r="E45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>41</v>
       </c>
@@ -8401,8 +8720,15 @@
       <c r="E46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>20</v>
       </c>
@@ -8418,8 +8744,15 @@
       <c r="E47">
         <v>0.47077970605330899</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47">
+        <v>0.47077970605330899</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>29</v>
       </c>
@@ -8435,8 +8768,15 @@
       <c r="E48">
         <v>2.93746218906062E-2</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48">
+        <v>2.93746218906062E-2</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>33</v>
       </c>
@@ -8452,8 +8792,15 @@
       <c r="E49">
         <v>0.210933717670411</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49">
+        <v>0.210933717670411</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>37</v>
       </c>
@@ -8469,8 +8816,15 @@
       <c r="E50">
         <v>0.214873251800097</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50">
+        <v>0.214873251800097</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>41</v>
       </c>
@@ -8486,8 +8840,15 @@
       <c r="E51">
         <v>7.4038702585576294E-2</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51">
+        <v>7.4038702585576294E-2</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>20</v>
       </c>
@@ -8503,8 +8864,15 @@
       <c r="E52">
         <v>0.99999682269713996</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52">
+        <v>0.99999682269713996</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>29</v>
       </c>
@@ -8520,8 +8888,15 @@
       <c r="E53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>33</v>
       </c>
@@ -8537,8 +8912,15 @@
       <c r="E54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>37</v>
       </c>
@@ -8554,8 +8936,15 @@
       <c r="E55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>41</v>
       </c>
@@ -8571,8 +8960,15 @@
       <c r="E56" s="1">
         <v>3.1773028597357298E-6</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56" s="1">
+        <v>3.1773028597357298E-6</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>20</v>
       </c>
@@ -8588,8 +8984,15 @@
       <c r="E57">
         <v>0.41934094839441899</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F57">
+        <v>0.41934094839441899</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>29</v>
       </c>
@@ -8605,8 +9008,15 @@
       <c r="E58">
         <v>3.7342579741576898E-2</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F58">
+        <v>3.7342579741576898E-2</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>33</v>
       </c>
@@ -8622,8 +9032,15 @@
       <c r="E59">
         <v>0.24377071984773999</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F59">
+        <v>0.24377071984773999</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>37</v>
       </c>
@@ -8639,8 +9056,15 @@
       <c r="E60">
         <v>0.225782714675485</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F60">
+        <v>0.225782714675485</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>41</v>
       </c>
@@ -8655,6 +9079,13 @@
       </c>
       <c r="E61">
         <v>7.3763037340777604E-2</v>
+      </c>
+      <c r="F61">
+        <v>7.3763037340777604E-2</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>